<commit_message>
sobe front com busca
</commit_message>
<xml_diff>
--- a/graduation-api/convidados_confirmados.xlsx
+++ b/graduation-api/convidados_confirmados.xlsx
@@ -400,20 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -446,6 +433,66 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
+        <v>Carlos Anderson Vargas da Silva</v>
+      </c>
+      <c r="C2" t="str">
+        <v>CRIANCA (40 anos)</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>1240</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Confirmado</v>
+      </c>
+      <c r="G2" t="str">
+        <v>19/04/2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>#</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Nome</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Tipo</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Idade</v>
+      </c>
+      <c r="E1" t="str">
+        <v>CodigoConvite</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="G1" t="str">
+        <v>DataConfirmacao</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
         <v>João Pedro Vargas da Silva</v>
       </c>
       <c r="C2" t="str">
@@ -487,32 +534,9 @@
         <v>19/04/2025</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Carlos Anderson Vargas da Silva</v>
-      </c>
-      <c r="C4" t="str">
-        <v>CRIANCA (40 anos)</v>
-      </c>
-      <c r="D4">
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <v>1240</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Recusado</v>
-      </c>
-      <c r="G4" t="str">
-        <v>19/04/2025</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -770,19 +794,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>8</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>